<commit_message>
Fix for return original
</commit_message>
<xml_diff>
--- a/common/file_templates/list_ss.xlsx
+++ b/common/file_templates/list_ss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\working\aa_dev\common\file_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52192C0D-0F16-4F6C-A226-91A52C09E52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5154906-D5C0-45F5-84CA-CAF7D6F0D60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Номер</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>[application.is_el_original_epk]</t>
+  </si>
+  <si>
+    <t>Забрал оригинал</t>
+  </si>
+  <si>
+    <t>[application.is_return_original_epk]</t>
   </si>
 </sst>
 </file>
@@ -277,13 +283,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -588,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE6"/>
+  <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -616,16 +625,16 @@
     <col min="18" max="20" width="22.73046875" customWidth="1"/>
     <col min="21" max="21" width="25.9296875" customWidth="1"/>
     <col min="22" max="22" width="23.86328125" customWidth="1"/>
-    <col min="23" max="24" width="25.86328125" customWidth="1"/>
-    <col min="25" max="25" width="22.86328125" customWidth="1"/>
-    <col min="26" max="26" width="28.06640625" customWidth="1"/>
-    <col min="27" max="27" width="27.59765625" customWidth="1"/>
-    <col min="28" max="28" width="24.73046875" customWidth="1"/>
-    <col min="29" max="29" width="32.73046875" customWidth="1"/>
-    <col min="30" max="30" width="31.19921875" customWidth="1"/>
+    <col min="23" max="25" width="25.86328125" customWidth="1"/>
+    <col min="26" max="26" width="22.86328125" customWidth="1"/>
+    <col min="27" max="27" width="28.06640625" customWidth="1"/>
+    <col min="28" max="28" width="27.59765625" customWidth="1"/>
+    <col min="29" max="29" width="24.73046875" customWidth="1"/>
+    <col min="30" max="30" width="32.73046875" customWidth="1"/>
+    <col min="31" max="31" width="31.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -698,29 +707,32 @@
       <c r="X1" t="s">
         <v>60</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z1" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -794,28 +806,31 @@
         <v>61</v>
       </c>
       <c r="Y2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
       <c r="C6" s="2"/>
     </row>
   </sheetData>

</xml_diff>